<commit_message>
Test avant suppression pic par excel
</commit_message>
<xml_diff>
--- a/SonarLysaFX/src/test/resources/lots_Pic.xlsx
+++ b/SonarLysaFX/src/test/resources/lots_Pic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="28515" windowHeight="13350" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="28515" windowHeight="13350"/>
   </bookViews>
   <sheets>
     <sheet name="E30" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7820" uniqueCount="3086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7829" uniqueCount="3087">
   <si>
     <t>N°</t>
   </si>
@@ -9278,6 +9278,9 @@
   </si>
   <si>
     <t>Installation - API CatalogueDesNomenclatures E32_ [NOM9 v1 - 15.00.00.00]</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -9619,11 +9622,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N574"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="131.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -9673,8 +9679,8 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>137977</v>
+      <c r="B2" t="s">
+        <v>3086</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -9714,8 +9720,8 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>195520</v>
+      <c r="B3" t="s">
+        <v>3086</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -9738,16 +9744,16 @@
       <c r="I3" s="1">
         <v>43054</v>
       </c>
-      <c r="N3" s="1">
-        <v>43054</v>
+      <c r="N3" s="1" t="s">
+        <v>3086</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>198676</v>
+      <c r="B4" t="s">
+        <v>3086</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -9778,6 +9784,9 @@
       </c>
       <c r="M4" s="1">
         <v>42781</v>
+      </c>
+      <c r="N4" t="s">
+        <v>3086</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -10009,8 +10018,8 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>224551</v>
+      <c r="B11" t="s">
+        <v>3086</v>
       </c>
       <c r="C11" t="s">
         <v>45</v>
@@ -10112,6 +10121,9 @@
       <c r="L13" s="1">
         <v>42928</v>
       </c>
+      <c r="N13" t="s">
+        <v>3086</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -10453,8 +10465,8 @@
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>238732</v>
+      <c r="B23" t="s">
+        <v>3086</v>
       </c>
       <c r="C23" t="s">
         <v>82</v>
@@ -10483,8 +10495,8 @@
       <c r="M23" s="1">
         <v>42909</v>
       </c>
-      <c r="N23" s="1">
-        <v>42975</v>
+      <c r="N23" s="1" t="s">
+        <v>3086</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -39144,8 +39156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>